<commit_message>
FEATURE: Economic Activity get dada from excell file
</commit_message>
<xml_diff>
--- a/src/eai/assets/report.xlsx
+++ b/src/eai/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>The EAI has a format error</t>
+    <t>Índices do Volume de Negócios: Invalid indicator sheet</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44826.64751933177</v>
+        <v>44827.56480612321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Economic Activity get all data
</commit_message>
<xml_diff>
--- a/src/eai/assets/report.xlsx
+++ b/src/eai/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Índices do Volume de Negócios: Invalid indicator sheet</t>
+    <t>aggregate Economic Activities Index: has a format error on indices do volume de negócios</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44827.64238668215</v>
+        <v>44827.70537058497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>